<commit_message>
Correcciones y finalización del proyecto
</commit_message>
<xml_diff>
--- a/companies.xlsx
+++ b/companies.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -37,43 +37,40 @@
     <t>Impact</t>
   </si>
   <si>
-    <t>Tech Solutions S.A.</t>
+    <t>plust ti</t>
   </si>
   <si>
     <t>Empresa de software innovador</t>
   </si>
   <si>
+    <t>contacto@plusti.com</t>
+  </si>
+  <si>
+    <t>987654327</t>
+  </si>
+  <si>
+    <t>av. principal 04-56, ciudad guatemala</t>
+  </si>
+  <si>
+    <t>desarrollo de software</t>
+  </si>
+  <si>
+    <t>10 años</t>
+  </si>
+  <si>
+    <t>multinacional</t>
+  </si>
+  <si>
+    <t>tech solutions s.a.</t>
+  </si>
+  <si>
     <t>contacto@techsolutions.com</t>
   </si>
   <si>
-    <t>987654321</t>
-  </si>
-  <si>
-    <t>Av. Principal 456, Ciudad Guatemala</t>
-  </si>
-  <si>
-    <t>Desarrollo de Software</t>
-  </si>
-  <si>
-    <t>15 años</t>
-  </si>
-  <si>
-    <t>Multinacional</t>
-  </si>
-  <si>
-    <t>Plust ti</t>
-  </si>
-  <si>
-    <t>contacto@plusti.com</t>
-  </si>
-  <si>
-    <t>987654322</t>
-  </si>
-  <si>
-    <t>Av. Principal 4-56, Ciudad Guatemala</t>
-  </si>
-  <si>
-    <t>11 años</t>
+    <t>987654325</t>
+  </si>
+  <si>
+    <t>av. principal 40-56, ciudad guatemala</t>
   </si>
 </sst>
 </file>
@@ -528,7 +525,7 @@
         <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>

</xml_diff>